<commit_message>
updates and adding a folder for invoices
</commit_message>
<xml_diff>
--- a/expenses_Paid.xlsx
+++ b/expenses_Paid.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Carlos Mariscal</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>NES controllers</t>
+  </si>
+  <si>
+    <t>digikey</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -428,6 +431,9 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
@@ -439,7 +445,9 @@
       <c r="C2" s="1">
         <v>11</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>33.83</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>

</xml_diff>

<commit_message>
link to programming AVR  (great resource)
</commit_message>
<xml_diff>
--- a/expenses_Paid.xlsx
+++ b/expenses_Paid.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Carlos Mariscal</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goodwill </t>
   </si>
 </sst>
 </file>
@@ -415,7 +418,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -434,6 +437,9 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
@@ -448,7 +454,9 @@
       <c r="D2" s="1">
         <v>33.83</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>

</xml_diff>